<commit_message>
lab 16 and additionali
vpa without hpa
</commit_message>
<xml_diff>
--- a/lab12/lab13сервер-сервер.xlsx
+++ b/lab12/lab13сервер-сервер.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kidawr/Desktop/Сириус/hl-module1/lab12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214343E-6053-AC4E-AAFF-1F12E28D9A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE85C8D0-24C0-404D-91DA-20BB501200E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>Количество ядер</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>50/50</t>
   </si>
@@ -34,10 +31,10 @@
     <t>Время в зависимости от запросов ppost%</t>
   </si>
   <si>
-    <t>lab13 2</t>
+    <t>lab16</t>
   </si>
   <si>
-    <t>lab13 1</t>
+    <t>наличие hpa</t>
   </si>
 </sst>
 </file>
@@ -86,12 +83,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -142,7 +142,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -157,10 +157,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8</c:v>
+                  <c:v>1.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -192,7 +192,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -207,10 +207,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -242,7 +242,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -257,10 +257,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,346 +269,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D79E-D24E-B919-5A94DC561A75}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1459188615"/>
-        <c:axId val="1767873414"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1459188615"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="ru-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1767873414"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1767873414"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="ru-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1459188615"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="4285F4"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$B$7:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$C$28:$C$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5C15-D245-A669-4E97FA2C240D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="EA4335"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$B$7:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$D$28:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5C15-D245-A669-4E97FA2C240D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FBBC04"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$B$7:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$E$28:$E$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>83</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5C15-D245-A669-4E97FA2C240D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -810,39 +470,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 1" title="Диаграмма">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DD130A9-87F4-DD4C-B08A-EA1D7E19DFA4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1054,8 +681,8 @@
   </sheetPr>
   <dimension ref="A5:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1065,13 +692,13 @@
   <sheetData>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1081,7 +708,7 @@
         <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -1089,36 +716,39 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>4.4000000000000004</v>
+        <v>3.5</v>
       </c>
       <c r="D7" s="1">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3.8</v>
+        <v>1.69</v>
       </c>
       <c r="D8" s="1">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>34.65</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1129,7 +759,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1140,56 +770,28 @@
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="1">
-        <v>95</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>5</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C28" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="D28" s="1">
-        <v>80</v>
-      </c>
-      <c r="E28" s="1">
-        <v>85</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D29" s="1">
-        <v>78</v>
-      </c>
-      <c r="E29" s="1">
-        <v>83</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="1"/>
@@ -1205,7 +807,7 @@
     </row>
     <row r="38" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E38" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>